<commit_message>
created plot for smeg growth curvewith added significance levels
</commit_message>
<xml_diff>
--- a/data/Processed_data/IA7_smeg_growth_curve.xlsx
+++ b/data/Processed_data/IA7_smeg_growth_curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ousstudent/Documents/Isma_Michael_summer2023/data/Processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A833DC1B-0D63-3748-BD99-FFC14D5AF81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95621A66-A8BB-4640-A1AA-A3747848C8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15440" xr2:uid="{3CDCA27F-3569-684E-97A6-4B0BA1EE9745}"/>
+    <workbookView xWindow="1160" yWindow="940" windowWidth="27640" windowHeight="15440" xr2:uid="{3CDCA27F-3569-684E-97A6-4B0BA1EE9745}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="12">
   <si>
     <t>od</t>
   </si>
@@ -33,13 +33,43 @@
     <t>condition</t>
   </si>
   <si>
-    <t>timepoint</t>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>1+</t>
+  </si>
+  <si>
+    <t>2+</t>
+  </si>
+  <si>
+    <t>3+</t>
+  </si>
+  <si>
+    <t>1-</t>
+  </si>
+  <si>
+    <t>2-</t>
+  </si>
+  <si>
+    <t>3-</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>vehicle</t>
+  </si>
+  <si>
+    <t>DPPC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -76,9 +106,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{693C3073-81E2-5A4C-A9CF-48D7FEDAC885}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -405,9 +436,9 @@
     <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -415,53 +446,596 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
       <c r="B3">
-        <v>2</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
       <c r="B4">
+        <v>0.255</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1.2749999999999999</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0.187</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="C12">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>0.86299999999999999</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1.198</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16">
+        <v>0.113</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <v>0.184</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>0.41</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <v>0.876</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22">
+        <v>1.2430000000000001</v>
+      </c>
+      <c r="C22">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="B23">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6">
+      <c r="B24">
+        <v>0.217</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>0.94099999999999995</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>1.33</v>
+      </c>
+      <c r="C29">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>0.12</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>0.623</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>1.24</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="B37">
+        <v>0.12</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7">
+      <c r="B38">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>6</v>
+      <c r="B39">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>0.628</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>0.876</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>1.2609999999999999</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>